<commit_message>
adapted cop computation for full model
</commit_message>
<xml_diff>
--- a/PythonResources/RunCases/seasonal_cop.xlsx
+++ b/PythonResources/RunCases/seasonal_cop.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="ETS_All_futu_monthly" sheetId="1" r:id="rId1"/>
-    <sheet name="ETS_All_futu_overall" sheetId="2" r:id="rId2"/>
+    <sheet name="ETS_1_monthly" sheetId="1" r:id="rId1"/>
+    <sheet name="ETS_1_overall" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>mode</t>
   </si>
@@ -32,16 +32,16 @@
     <t>COP_mon</t>
   </si>
   <si>
-    <t>TConEnt_avg</t>
-  </si>
-  <si>
-    <t>TConLvg_avg</t>
-  </si>
-  <si>
-    <t>TEvaEnt_avg</t>
-  </si>
-  <si>
-    <t>TEvaLvg_avg</t>
+    <t>TConEnt_avg|K</t>
+  </si>
+  <si>
+    <t>TConLvg_avg|K</t>
+  </si>
+  <si>
+    <t>TEvaEnt_avg|K</t>
+  </si>
+  <si>
+    <t>TEvaLvg_avg|K</t>
   </si>
   <si>
     <t>size</t>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Sep</t>
-  </si>
-  <si>
-    <t>COP_overall</t>
   </si>
 </sst>
 </file>
@@ -546,58 +543,40 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>8.260119438171387</v>
+        <v>7.942139933204688</v>
       </c>
       <c r="C4">
-        <v>302.2760314941406</v>
+        <v>304.3406020454739</v>
       </c>
       <c r="D4">
-        <v>305.134033203125</v>
+        <v>306.6870720904806</v>
       </c>
       <c r="E4">
-        <v>284.35693359375</v>
+        <v>284.7343922490659</v>
       </c>
       <c r="F4">
-        <v>281.893310546875</v>
+        <v>282.6839639414912</v>
       </c>
       <c r="G4">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="H4">
-        <v>4.236333847045898</v>
+        <v>4.577358531884396</v>
       </c>
       <c r="I4">
-        <v>320.2389526367188</v>
+        <v>313.0036964416504</v>
       </c>
       <c r="J4">
-        <v>326.02880859375</v>
+        <v>321.1116828918457</v>
       </c>
       <c r="K4">
-        <v>287.5927429199219</v>
+        <v>285.4331016540527</v>
       </c>
       <c r="L4">
-        <v>283.1658325195312</v>
+        <v>279.0946235656738</v>
       </c>
       <c r="M4">
-        <v>57</v>
-      </c>
-      <c r="N4">
-        <v>4.478368282318115</v>
-      </c>
-      <c r="O4">
-        <v>314.3594665527344</v>
-      </c>
-      <c r="P4">
-        <v>323.0051574707031</v>
-      </c>
-      <c r="Q4">
-        <v>287.0860595703125</v>
-      </c>
-      <c r="R4">
-        <v>280.3630065917969</v>
-      </c>
-      <c r="S4">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -605,40 +584,22 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>9.896656036376953</v>
+        <v>7.398032102648034</v>
       </c>
       <c r="C5">
-        <v>298.2617797851562</v>
+        <v>304.2139945194639</v>
       </c>
       <c r="D5">
-        <v>301.7628784179688</v>
+        <v>307.9323849382072</v>
       </c>
       <c r="E5">
-        <v>283.4510498046875</v>
+        <v>284.5940964271282</v>
       </c>
       <c r="F5">
-        <v>280.3036499023438</v>
+        <v>281.3789355047818</v>
       </c>
       <c r="G5">
-        <v>383</v>
-      </c>
-      <c r="N5">
-        <v>4.450370311737061</v>
-      </c>
-      <c r="O5">
-        <v>313.2778625488281</v>
-      </c>
-      <c r="P5">
-        <v>320.94970703125</v>
-      </c>
-      <c r="Q5">
-        <v>285.7809143066406</v>
-      </c>
-      <c r="R5">
-        <v>279.8245544433594</v>
-      </c>
-      <c r="S5">
-        <v>51</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -646,58 +607,40 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>3.860408067703247</v>
+        <v>7.178666154833804</v>
       </c>
       <c r="C6">
-        <v>326.66455078125</v>
+        <v>307.9058723449707</v>
       </c>
       <c r="D6">
-        <v>328.1434326171875</v>
+        <v>310.3665981292725</v>
       </c>
       <c r="E6">
-        <v>286.4805908203125</v>
+        <v>287.2326602935791</v>
       </c>
       <c r="F6">
-        <v>285.3741760253906</v>
+        <v>285.1433849334717</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="H6">
-        <v>4.034897327423096</v>
+        <v>3.74583039211916</v>
       </c>
       <c r="I6">
-        <v>324.9825744628906</v>
+        <v>320.0131688271799</v>
       </c>
       <c r="J6">
-        <v>328.186279296875</v>
+        <v>327.6829728977655</v>
       </c>
       <c r="K6">
-        <v>287.8526306152344</v>
+        <v>285.7267282137307</v>
       </c>
       <c r="L6">
-        <v>285.4390869140625</v>
+        <v>280.1015549526419</v>
       </c>
       <c r="M6">
-        <v>330</v>
-      </c>
-      <c r="N6">
-        <v>3.974022150039673</v>
-      </c>
-      <c r="O6">
-        <v>323.5985717773438</v>
-      </c>
-      <c r="P6">
-        <v>328.9264526367188</v>
-      </c>
-      <c r="Q6">
-        <v>287.2709655761719</v>
-      </c>
-      <c r="R6">
-        <v>283.2819213867188</v>
-      </c>
-      <c r="S6">
-        <v>14</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -705,58 +648,40 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>8.42600154876709</v>
+        <v>6.603569373483853</v>
       </c>
       <c r="C7">
-        <v>304.0924377441406</v>
+        <v>309.4853820800781</v>
       </c>
       <c r="D7">
-        <v>308.1418762207031</v>
+        <v>311.9534301757812</v>
       </c>
       <c r="E7">
-        <v>288.3482971191406</v>
+        <v>287.2582528250558</v>
       </c>
       <c r="F7">
-        <v>285.3430480957031</v>
+        <v>285.1903337751116</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>4.04999303817749</v>
+        <v>3.732659283004948</v>
       </c>
       <c r="I7">
-        <v>324.7951354980469</v>
+        <v>319.9744325295473</v>
       </c>
       <c r="J7">
-        <v>328.2342529296875</v>
+        <v>327.3189947666266</v>
       </c>
       <c r="K7">
-        <v>287.8313293457031</v>
+        <v>285.6676283616286</v>
       </c>
       <c r="L7">
-        <v>285.2379150390625</v>
+        <v>280.2876970340044</v>
       </c>
       <c r="M7">
-        <v>262</v>
-      </c>
-      <c r="N7">
-        <v>4.516412734985352</v>
-      </c>
-      <c r="O7">
-        <v>318.0373229980469</v>
-      </c>
-      <c r="P7">
-        <v>324.0388793945312</v>
-      </c>
-      <c r="Q7">
-        <v>287.3914184570312</v>
-      </c>
-      <c r="R7">
-        <v>282.7146606445312</v>
-      </c>
-      <c r="S7">
-        <v>14</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -764,58 +689,40 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>6.355806827545166</v>
+        <v>7.28299541021487</v>
       </c>
       <c r="C8">
-        <v>312.8745727539062</v>
+        <v>307.3153228759766</v>
       </c>
       <c r="D8">
-        <v>315.5295104980469</v>
+        <v>309.5024375915527</v>
       </c>
       <c r="E8">
-        <v>287.4021911621094</v>
+        <v>286.9843673706055</v>
       </c>
       <c r="F8">
-        <v>285.3552551269531</v>
+        <v>285.1379203796387</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="H8">
-        <v>3.907785415649414</v>
+        <v>3.577547628486173</v>
       </c>
       <c r="I8">
-        <v>326.3765258789062</v>
+        <v>321.2474238557635</v>
       </c>
       <c r="J8">
-        <v>329.2211608886719</v>
+        <v>329.1511213194649</v>
       </c>
       <c r="K8">
-        <v>287.89111328125</v>
+        <v>285.5648481261055</v>
       </c>
       <c r="L8">
-        <v>285.7737121582031</v>
+        <v>279.8674385502653</v>
       </c>
       <c r="M8">
-        <v>419</v>
-      </c>
-      <c r="N8">
-        <v>3.843437433242798</v>
-      </c>
-      <c r="O8">
-        <v>325.7818603515625</v>
-      </c>
-      <c r="P8">
-        <v>329.9517211914062</v>
-      </c>
-      <c r="Q8">
-        <v>287.5009155273438</v>
-      </c>
-      <c r="R8">
-        <v>284.416015625</v>
-      </c>
-      <c r="S8">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -823,40 +730,22 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>9.844882011413574</v>
+        <v>7.298668928368913</v>
       </c>
       <c r="C9">
-        <v>298.2466430664062</v>
+        <v>304.2545438228169</v>
       </c>
       <c r="D9">
-        <v>301.7916564941406</v>
+        <v>308.2897540899935</v>
       </c>
       <c r="E9">
-        <v>283.3627624511719</v>
+        <v>284.4730277775888</v>
       </c>
       <c r="F9">
-        <v>280.1774291992188</v>
+        <v>280.9909352159666</v>
       </c>
       <c r="G9">
-        <v>466</v>
-      </c>
-      <c r="N9">
-        <v>4.48253345489502</v>
-      </c>
-      <c r="O9">
-        <v>313.2931213378906</v>
-      </c>
-      <c r="P9">
-        <v>321.0192260742188</v>
-      </c>
-      <c r="Q9">
-        <v>285.809814453125</v>
-      </c>
-      <c r="R9">
-        <v>279.7855834960938</v>
-      </c>
-      <c r="S9">
-        <v>46</v>
+        <v>574</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -864,40 +753,22 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>9.678050994873047</v>
+        <v>7.495356099651389</v>
       </c>
       <c r="C10">
-        <v>298.4560852050781</v>
+        <v>304.2288258111299</v>
       </c>
       <c r="D10">
-        <v>301.8287353515625</v>
+        <v>307.6599715503294</v>
       </c>
       <c r="E10">
-        <v>283.3814697265625</v>
+        <v>284.5827935062238</v>
       </c>
       <c r="F10">
-        <v>280.3602294921875</v>
+        <v>281.6092470083664</v>
       </c>
       <c r="G10">
-        <v>288</v>
-      </c>
-      <c r="N10">
-        <v>4.517885208129883</v>
-      </c>
-      <c r="O10">
-        <v>313.8999328613281</v>
-      </c>
-      <c r="P10">
-        <v>321.6117553710938</v>
-      </c>
-      <c r="Q10">
-        <v>286.2642211914062</v>
-      </c>
-      <c r="R10">
-        <v>280.2542114257812</v>
-      </c>
-      <c r="S10">
-        <v>49</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -905,58 +776,58 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>5.938938140869141</v>
+        <v>7.398264981324923</v>
       </c>
       <c r="C11">
-        <v>311.09619140625</v>
+        <v>307.3450317382812</v>
       </c>
       <c r="D11">
-        <v>314.5847473144531</v>
+        <v>309.6193695068359</v>
       </c>
       <c r="E11">
-        <v>288.313720703125</v>
+        <v>287.0662892659505</v>
       </c>
       <c r="F11">
-        <v>285.3676147460938</v>
+        <v>285.1390635172526</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H11">
-        <v>4.128118991851807</v>
+        <v>3.903475843913796</v>
       </c>
       <c r="I11">
-        <v>323.3133850097656</v>
+        <v>318.3003565470378</v>
       </c>
       <c r="J11">
-        <v>327.3768920898438</v>
+        <v>325.9420687357585</v>
       </c>
       <c r="K11">
-        <v>287.7739562988281</v>
+        <v>285.6641527811686</v>
       </c>
       <c r="L11">
-        <v>284.6846618652344</v>
+        <v>279.9779968261719</v>
       </c>
       <c r="M11">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="N11">
-        <v>4.31077241897583</v>
+        <v>5.090269250889454</v>
       </c>
       <c r="O11">
-        <v>318.0433044433594</v>
+        <v>310.7619323730469</v>
       </c>
       <c r="P11">
-        <v>325.347900390625</v>
+        <v>319.2355041503906</v>
       </c>
       <c r="Q11">
-        <v>287.2880859375</v>
+        <v>287.1790466308594</v>
       </c>
       <c r="R11">
-        <v>281.6747131347656</v>
+        <v>280.3726196289062</v>
       </c>
       <c r="S11">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -964,58 +835,40 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>9.471240997314453</v>
+        <v>7.801118574982373</v>
       </c>
       <c r="C12">
-        <v>299.259033203125</v>
+        <v>304.2833319223055</v>
       </c>
       <c r="D12">
-        <v>302.3511657714844</v>
+        <v>307.0497262606057</v>
       </c>
       <c r="E12">
-        <v>283.4800415039062</v>
+        <v>284.9828753727738</v>
       </c>
       <c r="F12">
-        <v>280.7197265625</v>
+        <v>282.5713207285891</v>
       </c>
       <c r="G12">
-        <v>86</v>
+        <v>372</v>
       </c>
       <c r="H12">
-        <v>4.460976600646973</v>
+        <v>4.941688848859474</v>
       </c>
       <c r="I12">
-        <v>317.3967895507812</v>
+        <v>310.209716796875</v>
       </c>
       <c r="J12">
-        <v>324.0598754882812</v>
+        <v>319.3551025390625</v>
       </c>
       <c r="K12">
-        <v>287.5252380371094</v>
+        <v>285.4824066162109</v>
       </c>
       <c r="L12">
-        <v>282.3504943847656</v>
+        <v>278.1847839355469</v>
       </c>
       <c r="M12">
-        <v>16</v>
-      </c>
-      <c r="N12">
-        <v>4.402478694915771</v>
-      </c>
-      <c r="O12">
-        <v>314.5096435546875</v>
-      </c>
-      <c r="P12">
-        <v>322.5653991699219</v>
-      </c>
-      <c r="Q12">
-        <v>286.3384094238281</v>
-      </c>
-      <c r="R12">
-        <v>280.1065979003906</v>
-      </c>
-      <c r="S12">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1023,58 +876,58 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>8.061860084533691</v>
+        <v>8.092016102171307</v>
       </c>
       <c r="C13">
-        <v>304.2957763671875</v>
+        <v>304.6202873461174</v>
       </c>
       <c r="D13">
-        <v>307.1539001464844</v>
+        <v>306.7063894560843</v>
       </c>
       <c r="E13">
-        <v>285.68017578125</v>
+        <v>285.4050653631037</v>
       </c>
       <c r="F13">
-        <v>283.223388671875</v>
+        <v>283.580605246804</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="H13">
-        <v>4.148767471313477</v>
+        <v>4.106205733069801</v>
       </c>
       <c r="I13">
-        <v>323.3537902832031</v>
+        <v>316.8456132676866</v>
       </c>
       <c r="J13">
-        <v>327.336181640625</v>
+        <v>325.5143636067708</v>
       </c>
       <c r="K13">
-        <v>287.7829284667969</v>
+        <v>286.3556230333116</v>
       </c>
       <c r="L13">
-        <v>284.7568969726562</v>
+        <v>279.7928449842665</v>
       </c>
       <c r="M13">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="N13">
-        <v>4.417261600494385</v>
+        <v>4.390349511591186</v>
       </c>
       <c r="O13">
-        <v>315.5202026367188</v>
+        <v>315.6627960205078</v>
       </c>
       <c r="P13">
-        <v>323.0206604003906</v>
+        <v>325.0311431884766</v>
       </c>
       <c r="Q13">
-        <v>286.9206848144531</v>
+        <v>287.5096435546875</v>
       </c>
       <c r="R13">
-        <v>281.1089172363281</v>
+        <v>280.2787322998047</v>
       </c>
       <c r="S13">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1082,58 +935,40 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>9.090106010437012</v>
+        <v>8.022839834009444</v>
       </c>
       <c r="C14">
-        <v>301.1658935546875</v>
+        <v>304.4334746979095</v>
       </c>
       <c r="D14">
-        <v>304.1561889648438</v>
+        <v>306.843497140067</v>
       </c>
       <c r="E14">
-        <v>284.982421875</v>
+        <v>285.469965002039</v>
       </c>
       <c r="F14">
-        <v>282.3912048339844</v>
+        <v>283.362056857937</v>
       </c>
       <c r="G14">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="H14">
-        <v>4.179242134094238</v>
+        <v>4.621800966566261</v>
       </c>
       <c r="I14">
-        <v>321.4307556152344</v>
+        <v>313.1015973772322</v>
       </c>
       <c r="J14">
-        <v>326.4805603027344</v>
+        <v>322.3745727539062</v>
       </c>
       <c r="K14">
-        <v>287.6790771484375</v>
+        <v>286.5446428571428</v>
       </c>
       <c r="L14">
-        <v>283.8341064453125</v>
+        <v>279.2734069824219</v>
       </c>
       <c r="M14">
-        <v>59</v>
-      </c>
-      <c r="N14">
-        <v>4.413254737854004</v>
-      </c>
-      <c r="O14">
-        <v>315.5215759277344</v>
-      </c>
-      <c r="P14">
-        <v>323.3701782226562</v>
-      </c>
-      <c r="Q14">
-        <v>286.9038696289062</v>
-      </c>
-      <c r="R14">
-        <v>280.8279724121094</v>
-      </c>
-      <c r="S14">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1141,58 +976,40 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>10.03300762176514</v>
+        <v>7.631717645535224</v>
       </c>
       <c r="C15">
-        <v>298.2825622558594</v>
+        <v>304.2040211465122</v>
       </c>
       <c r="D15">
-        <v>301.5066528320312</v>
+        <v>307.3775184956772</v>
       </c>
       <c r="E15">
-        <v>283.3998107910156</v>
+        <v>284.7950769216528</v>
       </c>
       <c r="F15">
-        <v>280.4967041015625</v>
+        <v>282.0382810475137</v>
       </c>
       <c r="G15">
-        <v>201</v>
+        <v>422</v>
       </c>
       <c r="H15">
-        <v>4.475663185119629</v>
+        <v>7.728417475906985</v>
       </c>
       <c r="I15">
-        <v>318.2002868652344</v>
+        <v>307.4984741210937</v>
       </c>
       <c r="J15">
-        <v>324.2491149902344</v>
+        <v>310.1500244140625</v>
       </c>
       <c r="K15">
-        <v>287.5753479003906</v>
+        <v>289.1929016113281</v>
       </c>
       <c r="L15">
-        <v>282.8722534179688</v>
+        <v>286.8865051269531</v>
       </c>
       <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15">
-        <v>4.472246170043945</v>
-      </c>
-      <c r="O15">
-        <v>314.6073913574219</v>
-      </c>
-      <c r="P15">
-        <v>321.8884582519531</v>
-      </c>
-      <c r="Q15">
-        <v>286.3085327148438</v>
-      </c>
-      <c r="R15">
-        <v>280.6460876464844</v>
-      </c>
-      <c r="S15">
-        <v>56</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -1241,22 +1058,22 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4.420657157897949</v>
+        <v>4.697357491249054</v>
       </c>
       <c r="C2">
-        <v>286.5152587890625</v>
+        <v>287.3443450927734</v>
       </c>
       <c r="D2">
-        <v>280.7235717773438</v>
+        <v>280.3256759643555</v>
       </c>
       <c r="E2">
-        <v>315.3816528320312</v>
+        <v>313.2123641967773</v>
       </c>
       <c r="F2">
-        <v>322.856201171875</v>
+        <v>322.1333236694336</v>
       </c>
       <c r="G2">
-        <v>422</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1264,22 +1081,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.760165214538574</v>
+        <v>7.516163328096475</v>
       </c>
       <c r="C3">
-        <v>283.4704284667969</v>
+        <v>284.7888379355338</v>
       </c>
       <c r="D3">
-        <v>280.4186401367188</v>
+        <v>281.9301049682209</v>
       </c>
       <c r="E3">
-        <v>298.5841674804688</v>
+        <v>304.355131423593</v>
       </c>
       <c r="F3">
-        <v>301.988037109375</v>
+        <v>307.6541029710036</v>
       </c>
       <c r="G3">
-        <v>1482</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1287,22 +1104,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.06164026260376</v>
+        <v>3.820315707019815</v>
       </c>
       <c r="C4">
-        <v>287.8225708007812</v>
+        <v>285.753366388662</v>
       </c>
       <c r="D4">
-        <v>285.1519165039062</v>
+        <v>279.9777671371959</v>
       </c>
       <c r="E4">
-        <v>324.5692749023438</v>
+        <v>319.1527301778721</v>
       </c>
       <c r="F4">
-        <v>328.1075744628906</v>
+        <v>326.9720522018164</v>
       </c>
       <c r="G4">
-        <v>1459</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>